<commit_message>
Provide enumeration for library kit and flow cell
</commit_message>
<xml_diff>
--- a/user-interface/src/main/resources/templates/ngs_measurement_registration_sheet.xlsx
+++ b/user-interface/src/main/resources/templates/ngs_measurement_registration_sheet.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sven1103/git/data-manager/user-interface/src/main/resources/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{721FD578-451A-AF40-A2AF-5536DC7A3296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC0DD13-7416-C544-9FB1-12B94CF471EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-5500" windowWidth="38400" windowHeight="23500" xr2:uid="{D4F19D33-EE39-EF46-8DDD-2818EAD74D6D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{D4F19D33-EE39-EF46-8DDD-2818EAD74D6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
     <sheet name="Property information" sheetId="3" r:id="rId2"/>
     <sheet name="Allowed values" sheetId="2" r:id="rId3"/>
+    <sheet name="Library Kit - Info" sheetId="4" r:id="rId4"/>
+    <sheet name="Flow Cell - Info" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="94">
   <si>
     <t>facility</t>
   </si>
@@ -179,13 +181,154 @@
   </si>
   <si>
     <t>paired-end</t>
+  </si>
+  <si>
+    <t>SQK-16S024</t>
+  </si>
+  <si>
+    <t>SQK-DCS109</t>
+  </si>
+  <si>
+    <t>SQK-LRK001</t>
+  </si>
+  <si>
+    <t>SQK-LSK109</t>
+  </si>
+  <si>
+    <t>SQK-LSK109-XL</t>
+  </si>
+  <si>
+    <t>SQK-LSK110</t>
+  </si>
+  <si>
+    <t>SQK-NBD114-96</t>
+  </si>
+  <si>
+    <t>SQK-PBK004</t>
+  </si>
+  <si>
+    <t>SQK-PCB109</t>
+  </si>
+  <si>
+    <t>SQK-PCS109</t>
+  </si>
+  <si>
+    <t>SQK-PSK004</t>
+  </si>
+  <si>
+    <t>SQK-RAB204</t>
+  </si>
+  <si>
+    <t>SQK-RAD004</t>
+  </si>
+  <si>
+    <t>SQK-RBK004</t>
+  </si>
+  <si>
+    <t>SQK-RBK114-96</t>
+  </si>
+  <si>
+    <t>SQK-RNA002</t>
+  </si>
+  <si>
+    <t>SQK-RPB004</t>
+  </si>
+  <si>
+    <t>SQK-16S024 16S Barcoding Kit 1-24</t>
+  </si>
+  <si>
+    <t>SQK-DCS109 Direct cDNA Sequencing Kit</t>
+  </si>
+  <si>
+    <t>SQK-LRK001 Field Sequencing Kit</t>
+  </si>
+  <si>
+    <t>SQK-LSK109 Ligation Sequencing Kit</t>
+  </si>
+  <si>
+    <t>SQK-LSK109-XL Ligation Sequencing Kit XL</t>
+  </si>
+  <si>
+    <t>SQK-LSK110 Ligation Sequencing Kit</t>
+  </si>
+  <si>
+    <t>SQK-NBD114.96 Native Barcoding Kit 96</t>
+  </si>
+  <si>
+    <t>SQK-PBK004 PCR Barcoding Kit</t>
+  </si>
+  <si>
+    <t>SQK-PCB109 PCR-cDNA Barcoding Kit</t>
+  </si>
+  <si>
+    <t>SQK-PCS109 PCR-cDNA Sequencing Kit</t>
+  </si>
+  <si>
+    <t>SQK-PSK004 PCR Sequencing Kit</t>
+  </si>
+  <si>
+    <t>SQK-RAB204 16S Barcoding Kit</t>
+  </si>
+  <si>
+    <t>SQK-RAD004 Rapid Sequencing Kit</t>
+  </si>
+  <si>
+    <t>SQK-RBK004 Rapid Barcoding Kit</t>
+  </si>
+  <si>
+    <t>SQK-RBK114.96 Rapid Barcoding Kit 96</t>
+  </si>
+  <si>
+    <t>SQK-RNA002 Direct RNA Sequencing Kit</t>
+  </si>
+  <si>
+    <t>SQK-RPB004 Rapid PCR Barcoding Kit</t>
+  </si>
+  <si>
+    <t>Library Kit Code</t>
+  </si>
+  <si>
+    <t>Vendor</t>
+  </si>
+  <si>
+    <t>Oxford Nanopore Technologies</t>
+  </si>
+  <si>
+    <t>Flow Cell Code</t>
+  </si>
+  <si>
+    <t>FLO-FLG001</t>
+  </si>
+  <si>
+    <t>FLO-MIN106D</t>
+  </si>
+  <si>
+    <t>FLO-MIN111</t>
+  </si>
+  <si>
+    <t>FLO-MIN114</t>
+  </si>
+  <si>
+    <t>FLO-PRO002</t>
+  </si>
+  <si>
+    <t>FLO-PRO111</t>
+  </si>
+  <si>
+    <t>FLO-PRO114M</t>
+  </si>
+  <si>
+    <t>see Library Kit - Info</t>
+  </si>
+  <si>
+    <t>see Flow Cell - Info</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -219,6 +362,33 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -240,7 +410,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -249,7 +419,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -584,16 +758,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B69E707E-F04E-7B45-8A9B-6BA21F625A45}">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.83203125" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" customWidth="1"/>
     <col min="4" max="4" width="15.83203125" customWidth="1"/>
     <col min="5" max="5" width="22.5" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
@@ -633,120 +808,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="E2" t="s">
-        <v>46</v>
-      </c>
       <c r="J2" s="5"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="E3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="E4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="E5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="E6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="E7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="E8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="E9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="E10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="E11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="E12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="E13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="E14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="E15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="E16" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E17" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E18" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E19" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E20" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E21" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E22" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E23" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="24" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E24" t="s">
-        <v>45</v>
-      </c>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -757,12 +819,24 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E9FE736D-8162-4043-AE74-902320F56BCF}">
           <x14:formula1>
             <xm:f>'Allowed values'!$E$2:$E$3</xm:f>
           </x14:formula1>
           <xm:sqref>E1:E1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{253224FC-95D1-3941-9112-F8AA284EE1E6}">
+          <x14:formula1>
+            <xm:f>'Library Kit - Info'!$A$2:$A$18</xm:f>
+          </x14:formula1>
+          <xm:sqref>F1:F1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F7E108C3-2F48-4741-956B-FBC756BA7D71}">
+          <x14:formula1>
+            <xm:f>'Flow Cell - Info'!$A$2:$A$8</xm:f>
+          </x14:formula1>
+          <xm:sqref>G1:G1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -775,7 +849,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -913,10 +987,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CA9A15C-9427-F34B-B818-4D616E8AFF0A}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -926,12 +1000,14 @@
     <col min="3" max="3" width="18.6640625" customWidth="1"/>
     <col min="4" max="4" width="35.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.6640625" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.83203125" customWidth="1"/>
     <col min="9" max="9" width="16.6640625" customWidth="1"/>
     <col min="10" max="10" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -963,52 +1039,625 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="C2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K2" s="7"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="7"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="7"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="7"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="7"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="7"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="7"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="7"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="7"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="7"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="7"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="7"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="7"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="7"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="7"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="7"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="7"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13E0810B-3684-C647-8DE8-9A2ADA571E17}">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="33.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE236AFD-902B-1E45-9BAF-304A9B303153}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="27.1640625" customWidth="1"/>
+    <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>85</v>
+      </c>
       <c r="C2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" t="s">
-        <v>45</v>
-      </c>
-      <c r="J2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" t="s">
-        <v>29</v>
-      </c>
-      <c r="J4" s="6"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="D5" t="s">
-        <v>30</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C8" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove prefill from template
</commit_message>
<xml_diff>
--- a/user-interface/src/main/resources/templates/ngs_measurement_registration_sheet.xlsx
+++ b/user-interface/src/main/resources/templates/ngs_measurement_registration_sheet.xlsx
@@ -1,19 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steff\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE26E03C-D609-4D69-9323-12717A6CE5DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Metadata" sheetId="1" r:id="rId4"/>
-    <sheet name="Property information" sheetId="2" r:id="rId5"/>
-    <sheet name="Allowed-Values" sheetId="3" r:id="rId6"/>
+    <sheet name="Metadata" sheetId="1" r:id="rId1"/>
+    <sheet name="Property information" sheetId="2" r:id="rId2"/>
+    <sheet name="Allowed-Values" sheetId="3" r:id="rId3"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="55">
   <si>
     <t>QBIC sample ids*</t>
   </si>
@@ -57,166 +66,16 @@
     <t>Q007V001AM</t>
   </si>
   <si>
-    <t>This will be ignored 1</t>
-  </si>
-  <si>
-    <t>https://ror.org/02jx3x895</t>
-  </si>
-  <si>
-    <t>ITSS</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C62343</t>
-  </si>
-  <si>
-    <t>I have become reading 1</t>
-  </si>
-  <si>
-    <t>Billy the kit 1</t>
-  </si>
-  <si>
-    <t>Go with the flow 1</t>
-  </si>
-  <si>
-    <t>Fly you fools 1</t>
-  </si>
-  <si>
-    <t>My awesome index7 1</t>
-  </si>
-  <si>
-    <t>My awesome index5 1</t>
-  </si>
-  <si>
-    <t>Keep it noted 1</t>
-  </si>
-  <si>
     <t>Q007V002AU</t>
   </si>
   <si>
-    <t>This will be ignored 2</t>
-  </si>
-  <si>
-    <t>https://ror.org/02jx3x896</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C62344</t>
-  </si>
-  <si>
-    <t>I have become reading 2</t>
-  </si>
-  <si>
-    <t>Billy the kit 2</t>
-  </si>
-  <si>
-    <t>Go with the flow 2</t>
-  </si>
-  <si>
-    <t>Fly you fools 2</t>
-  </si>
-  <si>
-    <t>My awesome index7 2</t>
-  </si>
-  <si>
-    <t>My awesome index5 2</t>
-  </si>
-  <si>
-    <t>Keep it noted 2</t>
-  </si>
-  <si>
     <t>Q007V004AC</t>
   </si>
   <si>
-    <t>This will be ignored 3</t>
-  </si>
-  <si>
-    <t>https://ror.org/02jx3x897</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C62345</t>
-  </si>
-  <si>
-    <t>I have become reading 3</t>
-  </si>
-  <si>
-    <t>Billy the kit 3</t>
-  </si>
-  <si>
-    <t>Go with the flow 3</t>
-  </si>
-  <si>
-    <t>Fly you fools 3</t>
-  </si>
-  <si>
-    <t>My awesome index7 3</t>
-  </si>
-  <si>
-    <t>My awesome index5 3</t>
-  </si>
-  <si>
-    <t>Keep it noted 3</t>
-  </si>
-  <si>
     <t>Q007V003A4</t>
   </si>
   <si>
-    <t>This will be ignored 4</t>
-  </si>
-  <si>
-    <t>https://ror.org/02jx3x898</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C62346</t>
-  </si>
-  <si>
-    <t>I have become reading 4</t>
-  </si>
-  <si>
-    <t>Billy the kit 4</t>
-  </si>
-  <si>
-    <t>Go with the flow 4</t>
-  </si>
-  <si>
-    <t>Fly you fools 4</t>
-  </si>
-  <si>
-    <t>My awesome index7 4</t>
-  </si>
-  <si>
-    <t>My awesome index5 4</t>
-  </si>
-  <si>
-    <t>Keep it noted 4</t>
-  </si>
-  <si>
     <t>Q007V005AK</t>
-  </si>
-  <si>
-    <t>This will be ignored 5</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C62347</t>
-  </si>
-  <si>
-    <t>I have become reading 5</t>
-  </si>
-  <si>
-    <t>Billy the kit 5</t>
-  </si>
-  <si>
-    <t>Go with the flow 5</t>
-  </si>
-  <si>
-    <t>Fly you fools 5</t>
-  </si>
-  <si>
-    <t>My awesome index7 5</t>
-  </si>
-  <si>
-    <t>My awesome index5 5</t>
-  </si>
-  <si>
-    <t>Keep it noted 5</t>
   </si>
   <si>
     <t>Measurement Property</t>
@@ -333,28 +192,15 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Aptos Narrow"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="15"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="1"/>
+      <b/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
@@ -365,7 +211,7 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Arial"/>
@@ -460,71 +306,29 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+  </cellStyleXfs>
+  <cellXfs count="18">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-  </cellStyleXfs>
-  <cellXfs count="20">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -533,25 +337,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ffa7a7a7"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="FFA7A7A7"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -753,7 +617,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -771,7 +635,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -800,7 +664,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -825,7 +689,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -850,7 +714,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -875,7 +739,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -900,7 +764,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -925,7 +789,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -950,7 +814,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -975,7 +839,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1000,7 +864,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1013,9 +877,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -1032,7 +902,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1050,7 +920,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1075,7 +945,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1100,7 +970,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1125,7 +995,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1150,7 +1020,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1175,7 +1045,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1200,7 +1070,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1225,7 +1095,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1250,7 +1120,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1275,7 +1145,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1288,9 +1158,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1304,7 +1180,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1322,7 +1198,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1351,7 +1227,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1376,7 +1252,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1401,7 +1277,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1426,7 +1302,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1451,7 +1327,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1476,7 +1352,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1501,7 +1377,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1526,7 +1402,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1551,7 +1427,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1564,283 +1440,173 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8333" defaultRowHeight="16" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.1719" style="1" customWidth="1"/>
-    <col min="2" max="3" width="23.6719" style="1" customWidth="1"/>
+    <col min="1" max="1" width="29.125" style="1" customWidth="1"/>
+    <col min="2" max="3" width="23.625" style="1" customWidth="1"/>
     <col min="4" max="4" width="20.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.8516" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.875" style="1" customWidth="1"/>
     <col min="6" max="6" width="22.5" style="1" customWidth="1"/>
-    <col min="7" max="8" width="10.8516" style="1" customWidth="1"/>
+    <col min="7" max="8" width="10.875" style="1" customWidth="1"/>
     <col min="9" max="10" width="26" style="1" customWidth="1"/>
-    <col min="11" max="12" width="10.8516" style="1" customWidth="1"/>
-    <col min="13" max="13" width="101.352" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="10.8516" style="1" customWidth="1"/>
+    <col min="11" max="12" width="10.875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="101.375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="10.875" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.55" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="2">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="2">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="2">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s" s="2">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s" s="2">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s" s="2">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s" s="2">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s" s="2">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s" s="2">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" ht="17" customHeight="1">
-      <c r="A2" t="s" s="3">
+    <row r="2" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s" s="3">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+    </row>
+    <row r="3" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C2" t="s" s="3">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+    </row>
+    <row r="4" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D2" t="s" s="3">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+    </row>
+    <row r="5" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E2" t="s" s="3">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+    </row>
+    <row r="6" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F2" t="s" s="3">
-        <v>18</v>
-      </c>
-      <c r="G2" t="s" s="3">
-        <v>19</v>
-      </c>
-      <c r="H2" t="s" s="3">
-        <v>20</v>
-      </c>
-      <c r="I2" t="s" s="3">
-        <v>21</v>
-      </c>
-      <c r="J2" s="4">
-        <v>1</v>
-      </c>
-      <c r="K2" t="s" s="3">
-        <v>22</v>
-      </c>
-      <c r="L2" t="s" s="3">
-        <v>23</v>
-      </c>
-      <c r="M2" t="s" s="3">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" ht="17" customHeight="1">
-      <c r="A3" t="s" s="3">
-        <v>25</v>
-      </c>
-      <c r="B3" t="s" s="3">
-        <v>26</v>
-      </c>
-      <c r="C3" t="s" s="3">
-        <v>27</v>
-      </c>
-      <c r="D3" t="s" s="3">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s" s="3">
-        <v>28</v>
-      </c>
-      <c r="F3" t="s" s="3">
-        <v>29</v>
-      </c>
-      <c r="G3" t="s" s="3">
-        <v>30</v>
-      </c>
-      <c r="H3" t="s" s="3">
-        <v>31</v>
-      </c>
-      <c r="I3" t="s" s="3">
-        <v>32</v>
-      </c>
-      <c r="J3" s="4">
-        <v>2</v>
-      </c>
-      <c r="K3" t="s" s="3">
-        <v>33</v>
-      </c>
-      <c r="L3" t="s" s="3">
-        <v>34</v>
-      </c>
-      <c r="M3" t="s" s="3">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" ht="17" customHeight="1">
-      <c r="A4" t="s" s="3">
-        <v>36</v>
-      </c>
-      <c r="B4" t="s" s="3">
-        <v>37</v>
-      </c>
-      <c r="C4" t="s" s="3">
-        <v>38</v>
-      </c>
-      <c r="D4" t="s" s="3">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s" s="3">
-        <v>39</v>
-      </c>
-      <c r="F4" t="s" s="3">
-        <v>40</v>
-      </c>
-      <c r="G4" t="s" s="3">
-        <v>41</v>
-      </c>
-      <c r="H4" t="s" s="3">
-        <v>42</v>
-      </c>
-      <c r="I4" t="s" s="3">
-        <v>43</v>
-      </c>
-      <c r="J4" s="4">
-        <v>2</v>
-      </c>
-      <c r="K4" t="s" s="3">
-        <v>44</v>
-      </c>
-      <c r="L4" t="s" s="3">
-        <v>45</v>
-      </c>
-      <c r="M4" t="s" s="3">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" ht="17" customHeight="1">
-      <c r="A5" t="s" s="3">
-        <v>47</v>
-      </c>
-      <c r="B5" t="s" s="3">
-        <v>48</v>
-      </c>
-      <c r="C5" t="s" s="3">
-        <v>49</v>
-      </c>
-      <c r="D5" t="s" s="3">
-        <v>16</v>
-      </c>
-      <c r="E5" t="s" s="3">
-        <v>50</v>
-      </c>
-      <c r="F5" t="s" s="3">
-        <v>51</v>
-      </c>
-      <c r="G5" t="s" s="3">
-        <v>52</v>
-      </c>
-      <c r="H5" t="s" s="3">
-        <v>53</v>
-      </c>
-      <c r="I5" t="s" s="3">
-        <v>54</v>
-      </c>
-      <c r="J5" s="4">
-        <v>3</v>
-      </c>
-      <c r="K5" t="s" s="3">
-        <v>55</v>
-      </c>
-      <c r="L5" t="s" s="3">
-        <v>56</v>
-      </c>
-      <c r="M5" t="s" s="3">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" ht="17" customHeight="1">
-      <c r="A6" t="s" s="3">
-        <v>58</v>
-      </c>
-      <c r="B6" t="s" s="3">
-        <v>59</v>
-      </c>
-      <c r="C6" t="s" s="3">
-        <v>15</v>
-      </c>
-      <c r="D6" t="s" s="3">
-        <v>16</v>
-      </c>
-      <c r="E6" t="s" s="3">
-        <v>60</v>
-      </c>
-      <c r="F6" t="s" s="3">
-        <v>61</v>
-      </c>
-      <c r="G6" t="s" s="3">
-        <v>62</v>
-      </c>
-      <c r="H6" t="s" s="3">
-        <v>63</v>
-      </c>
-      <c r="I6" t="s" s="3">
-        <v>64</v>
-      </c>
-      <c r="J6" s="4">
-        <v>1</v>
-      </c>
-      <c r="K6" t="s" s="3">
-        <v>65</v>
-      </c>
-      <c r="L6" t="s" s="3">
-        <v>66</v>
-      </c>
-      <c r="M6" t="s" s="3">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" ht="17" customHeight="1">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+    </row>
+    <row r="7" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -1855,7 +1621,7 @@
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
     </row>
-    <row r="8" ht="17" customHeight="1">
+    <row r="8" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -1870,7 +1636,7 @@
       <c r="L8" s="8"/>
       <c r="M8" s="8"/>
     </row>
-    <row r="9" ht="17" customHeight="1">
+    <row r="9" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -1885,7 +1651,7 @@
       <c r="L9" s="8"/>
       <c r="M9" s="8"/>
     </row>
-    <row r="10" ht="17" customHeight="1">
+    <row r="10" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -1902,12 +1668,12 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F7:F10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F7:F10" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"single-end,paired-end"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -1915,204 +1681,204 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8333" defaultRowHeight="16" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="21.1719" style="11" customWidth="1"/>
-    <col min="3" max="3" width="86.1719" style="11" customWidth="1"/>
-    <col min="4" max="5" width="10.8516" style="11" customWidth="1"/>
-    <col min="6" max="16384" width="10.8516" style="11" customWidth="1"/>
+    <col min="1" max="2" width="21.125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="86.125" style="1" customWidth="1"/>
+    <col min="4" max="6" width="10.875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="17" customHeight="1">
-      <c r="A1" t="s" s="12">
-        <v>68</v>
-      </c>
-      <c r="B1" t="s" s="12">
-        <v>69</v>
-      </c>
-      <c r="C1" t="s" s="12">
-        <v>70</v>
+    <row r="1" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>20</v>
       </c>
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
     </row>
-    <row r="2" ht="26.55" customHeight="1">
-      <c r="A2" t="s" s="13">
-        <v>71</v>
-      </c>
-      <c r="B2" t="s" s="13">
-        <v>72</v>
-      </c>
-      <c r="C2" t="s" s="14">
-        <v>73</v>
+    <row r="2" spans="1:5" ht="26.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>23</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" ht="26.55" customHeight="1">
-      <c r="A3" t="s" s="13">
+    <row r="3" spans="1:5" ht="26.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s" s="13">
-        <v>74</v>
-      </c>
-      <c r="C3" t="s" s="14">
-        <v>75</v>
+      <c r="B3" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>25</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
     </row>
-    <row r="4" ht="26.55" customHeight="1">
-      <c r="A4" t="s" s="13">
-        <v>76</v>
-      </c>
-      <c r="B4" t="s" s="13">
-        <v>72</v>
-      </c>
-      <c r="C4" t="s" s="14">
-        <v>77</v>
+    <row r="4" spans="1:5" ht="26.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>27</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" ht="17" customHeight="1">
-      <c r="A5" t="s" s="13">
-        <v>78</v>
-      </c>
-      <c r="B5" t="s" s="13">
-        <v>72</v>
-      </c>
-      <c r="C5" t="s" s="14">
-        <v>79</v>
+    <row r="5" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>29</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
     </row>
-    <row r="6" ht="39.55" customHeight="1">
-      <c r="A6" t="s" s="13">
-        <v>80</v>
-      </c>
-      <c r="B6" t="s" s="13">
-        <v>72</v>
-      </c>
-      <c r="C6" t="s" s="14">
-        <v>81</v>
+    <row r="6" spans="1:5" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>31</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
     </row>
-    <row r="7" ht="17" customHeight="1">
-      <c r="A7" t="s" s="13">
-        <v>82</v>
-      </c>
-      <c r="B7" t="s" s="13">
-        <v>72</v>
-      </c>
-      <c r="C7" t="s" s="14">
-        <v>83</v>
+    <row r="7" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
     </row>
-    <row r="8" ht="26.55" customHeight="1">
-      <c r="A8" t="s" s="13">
+    <row r="8" spans="1:5" ht="26.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B8" t="s" s="13">
-        <v>74</v>
-      </c>
-      <c r="C8" t="s" s="14">
-        <v>84</v>
+      <c r="B8" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>34</v>
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
     </row>
-    <row r="9" ht="17" customHeight="1">
-      <c r="A9" t="s" s="13">
+    <row r="9" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B9" t="s" s="13">
-        <v>74</v>
-      </c>
-      <c r="C9" t="s" s="14">
-        <v>85</v>
+      <c r="B9" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>35</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
     </row>
-    <row r="10" ht="17" customHeight="1">
-      <c r="A10" t="s" s="13">
+    <row r="10" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B10" t="s" s="13">
-        <v>74</v>
-      </c>
-      <c r="C10" t="s" s="14">
-        <v>86</v>
+      <c r="B10" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>36</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
     </row>
-    <row r="11" ht="17" customHeight="1">
-      <c r="A11" t="s" s="13">
+    <row r="11" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B11" t="s" s="13">
-        <v>74</v>
-      </c>
-      <c r="C11" t="s" s="14">
-        <v>87</v>
+      <c r="B11" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>37</v>
       </c>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
     </row>
-    <row r="12" ht="17" customHeight="1">
-      <c r="A12" t="s" s="13">
+    <row r="12" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B12" t="s" s="14">
-        <v>74</v>
-      </c>
-      <c r="C12" t="s" s="14">
-        <v>88</v>
+      <c r="B12" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>38</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
     </row>
-    <row r="13" ht="17" customHeight="1">
-      <c r="A13" t="s" s="13">
+    <row r="13" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B13" t="s" s="14">
-        <v>74</v>
-      </c>
-      <c r="C13" t="s" s="14">
-        <v>88</v>
+      <c r="B13" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>38</v>
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
     </row>
-    <row r="14" ht="17" customHeight="1">
-      <c r="A14" t="s" s="13">
+    <row r="14" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B14" t="s" s="13">
-        <v>74</v>
-      </c>
-      <c r="C14" t="s" s="14">
-        <v>89</v>
+      <c r="B14" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>39</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -2120,139 +1886,142 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8333" defaultRowHeight="16" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.3516" style="15" customWidth="1"/>
-    <col min="2" max="3" width="16" style="15" customWidth="1"/>
-    <col min="4" max="4" width="18.6719" style="15" customWidth="1"/>
-    <col min="5" max="5" width="35.8516" style="15" customWidth="1"/>
-    <col min="6" max="6" width="26.6719" style="15" customWidth="1"/>
-    <col min="7" max="7" width="15.3516" style="15" customWidth="1"/>
-    <col min="8" max="8" width="14.8516" style="15" customWidth="1"/>
-    <col min="9" max="9" width="22.8516" style="15" customWidth="1"/>
-    <col min="10" max="10" width="19.1719" style="15" customWidth="1"/>
-    <col min="11" max="12" width="16.6719" style="15" customWidth="1"/>
-    <col min="13" max="13" width="24" style="15" customWidth="1"/>
-    <col min="14" max="16384" width="10.8516" style="15" customWidth="1"/>
+    <col min="1" max="1" width="30.375" style="1" customWidth="1"/>
+    <col min="2" max="3" width="16" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="35.875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="26.625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="22.875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="19.125" style="1" customWidth="1"/>
+    <col min="11" max="12" width="16.625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="24" style="1" customWidth="1"/>
+    <col min="14" max="14" width="10.875" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.55" customHeight="1">
-      <c r="A1" t="s" s="16">
-        <v>90</v>
-      </c>
-      <c r="B1" t="s" s="16">
+    <row r="1" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="16">
+      <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="16">
+      <c r="D1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="16">
+      <c r="E1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="16">
+      <c r="F1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="16">
+      <c r="G1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s" s="16">
+      <c r="H1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s" s="16">
+      <c r="I1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s" s="16">
+      <c r="J1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s" s="16">
+      <c r="K1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s" s="16">
+      <c r="L1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s" s="16">
+      <c r="M1" s="14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" ht="13.55" customHeight="1">
-      <c r="A2" t="s" s="13">
-        <v>91</v>
-      </c>
-      <c r="B2" t="s" s="13">
-        <v>92</v>
-      </c>
-      <c r="C2" t="s" s="13">
-        <v>93</v>
-      </c>
-      <c r="D2" t="s" s="13">
-        <v>94</v>
-      </c>
-      <c r="E2" t="s" s="13">
-        <v>95</v>
-      </c>
-      <c r="F2" t="s" s="13">
-        <v>96</v>
-      </c>
-      <c r="G2" t="s" s="13">
-        <v>92</v>
-      </c>
-      <c r="H2" t="s" s="13">
-        <v>92</v>
-      </c>
-      <c r="I2" t="s" s="13">
-        <v>92</v>
-      </c>
-      <c r="J2" t="s" s="17">
-        <v>97</v>
-      </c>
-      <c r="K2" t="s" s="13">
-        <v>92</v>
-      </c>
-      <c r="L2" t="s" s="13">
-        <v>92</v>
-      </c>
-      <c r="M2" t="s" s="13">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" t="s" s="13">
-        <v>99</v>
-      </c>
-      <c r="B3" s="13"/>
-      <c r="C3" t="s" s="13">
-        <v>100</v>
+    <row r="2" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="J2" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="L2" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="M2" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12" t="s">
+        <v>50</v>
       </c>
       <c r="D3" s="10"/>
-      <c r="E3" t="s" s="13">
-        <v>101</v>
-      </c>
-      <c r="F3" t="s" s="13">
-        <v>102</v>
+      <c r="E3" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>52</v>
       </c>
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
-      <c r="J3" s="13"/>
+      <c r="J3" s="12"/>
       <c r="K3" s="10"/>
       <c r="L3" s="10"/>
       <c r="M3" s="10"/>
     </row>
-    <row r="4" ht="13.55" customHeight="1">
+    <row r="4" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
-      <c r="E4" t="s" s="13">
-        <v>103</v>
+      <c r="E4" s="12" t="s">
+        <v>53</v>
       </c>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
@@ -2261,15 +2030,15 @@
       <c r="J4" s="10"/>
       <c r="K4" s="10"/>
       <c r="L4" s="10"/>
-      <c r="M4" s="18"/>
-    </row>
-    <row r="5" ht="13.55" customHeight="1">
+      <c r="M4" s="16"/>
+    </row>
+    <row r="5" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
-      <c r="E5" t="s" s="13">
-        <v>104</v>
+      <c r="E5" s="12" t="s">
+        <v>54</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
@@ -2280,7 +2049,7 @@
       <c r="L5" s="10"/>
       <c r="M5" s="10"/>
     </row>
-    <row r="6" ht="13.55" customHeight="1">
+    <row r="6" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10"/>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
@@ -2295,7 +2064,7 @@
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
     </row>
-    <row r="7" ht="13.55" customHeight="1">
+    <row r="7" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
@@ -2310,7 +2079,7 @@
       <c r="L7" s="10"/>
       <c r="M7" s="10"/>
     </row>
-    <row r="8" ht="13.55" customHeight="1">
+    <row r="8" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
@@ -2325,7 +2094,7 @@
       <c r="L8" s="10"/>
       <c r="M8" s="10"/>
     </row>
-    <row r="9" ht="13.55" customHeight="1">
+    <row r="9" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
@@ -2340,7 +2109,7 @@
       <c r="L9" s="10"/>
       <c r="M9" s="10"/>
     </row>
-    <row r="10" ht="13.55" customHeight="1">
+    <row r="10" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
@@ -2355,7 +2124,7 @@
       <c r="L10" s="10"/>
       <c r="M10" s="10"/>
     </row>
-    <row r="11" ht="13.55" customHeight="1">
+    <row r="11" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
@@ -2370,7 +2139,7 @@
       <c r="L11" s="10"/>
       <c r="M11" s="10"/>
     </row>
-    <row r="12" ht="13.55" customHeight="1">
+    <row r="12" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
@@ -2385,7 +2154,7 @@
       <c r="L12" s="10"/>
       <c r="M12" s="10"/>
     </row>
-    <row r="13" ht="13.55" customHeight="1">
+    <row r="13" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
@@ -2400,7 +2169,7 @@
       <c r="L13" s="10"/>
       <c r="M13" s="10"/>
     </row>
-    <row r="14" ht="13.55" customHeight="1">
+    <row r="14" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
@@ -2415,7 +2184,7 @@
       <c r="L14" s="10"/>
       <c r="M14" s="10"/>
     </row>
-    <row r="15" ht="13.55" customHeight="1">
+    <row r="15" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
@@ -2430,7 +2199,7 @@
       <c r="L15" s="10"/>
       <c r="M15" s="10"/>
     </row>
-    <row r="16" ht="13.55" customHeight="1">
+    <row r="16" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
@@ -2445,7 +2214,7 @@
       <c r="L16" s="10"/>
       <c r="M16" s="10"/>
     </row>
-    <row r="17" ht="13.55" customHeight="1">
+    <row r="17" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10"/>
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
@@ -2460,7 +2229,7 @@
       <c r="L17" s="10"/>
       <c r="M17" s="10"/>
     </row>
-    <row r="18" ht="13.55" customHeight="1">
+    <row r="18" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
@@ -2475,84 +2244,84 @@
       <c r="L18" s="10"/>
       <c r="M18" s="10"/>
     </row>
-    <row r="19" ht="16" customHeight="1">
-      <c r="A19" s="19"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="19"/>
-      <c r="K19" s="19"/>
-      <c r="L19" s="19"/>
-      <c r="M19" s="19"/>
-    </row>
-    <row r="20" ht="16" customHeight="1">
-      <c r="A20" s="19"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="19"/>
-      <c r="K20" s="19"/>
-      <c r="L20" s="19"/>
-      <c r="M20" s="19"/>
-    </row>
-    <row r="21" ht="16" customHeight="1">
-      <c r="A21" s="19"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="19"/>
-      <c r="J21" s="19"/>
-      <c r="K21" s="19"/>
-      <c r="L21" s="19"/>
-      <c r="M21" s="19"/>
-    </row>
-    <row r="22" ht="16" customHeight="1">
-      <c r="A22" s="19"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
-      <c r="J22" s="19"/>
-      <c r="K22" s="19"/>
-      <c r="L22" s="19"/>
-      <c r="M22" s="19"/>
-    </row>
-    <row r="23" ht="16" customHeight="1">
-      <c r="A23" s="19"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="19"/>
-      <c r="J23" s="19"/>
-      <c r="K23" s="19"/>
-      <c r="L23" s="19"/>
-      <c r="M23" s="19"/>
+    <row r="19" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="17"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="17"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="17"/>
+    </row>
+    <row r="20" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="17"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="17"/>
+      <c r="L20" s="17"/>
+      <c r="M20" s="17"/>
+    </row>
+    <row r="21" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="17"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="17"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="17"/>
+    </row>
+    <row r="22" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="17"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="17"/>
+      <c r="K22" s="17"/>
+      <c r="L22" s="17"/>
+      <c r="M22" s="17"/>
+    </row>
+    <row r="23" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="17"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17"/>
+      <c r="K23" s="17"/>
+      <c r="L23" s="17"/>
+      <c r="M23" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
replace remaining 'code' and fix plural for spreadsheets
</commit_message>
<xml_diff>
--- a/user-interface/src/main/resources/templates/ngs_measurement_registration_sheet.xlsx
+++ b/user-interface/src/main/resources/templates/ngs_measurement_registration_sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sven1103/git/data-manager/user-interface/src/main/resources/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/afriedrich/git/data-manager-app/user-interface/src/main/resources/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95CEBC0B-66F3-B142-A89B-9CF57FB4E8AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44060A07-D260-904A-9ABB-310DB2F9189F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{D4F19D33-EE39-EF46-8DDD-2818EAD74D6D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{D4F19D33-EE39-EF46-8DDD-2818EAD74D6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="96">
   <si>
     <t>facility</t>
   </si>
@@ -325,6 +325,9 @@
   </si>
   <si>
     <t>index i7</t>
+  </si>
+  <si>
+    <t>QBIC sample ids</t>
   </si>
 </sst>
 </file>
@@ -995,9 +998,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CA9A15C-9427-F34B-B818-4D616E8AFF0A}">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1015,7 +1016,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>2</v>
+        <v>95</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Use 'ID' instead of 'Code' in the UI (#536)
* Use 'ID' instead of 'Code' in UI

* replace remaining 'code' and fix plural for spreadsheets

* adapt test

---------

Co-authored-by: Steffengreiner <steffen.greiner@qbic.uni-tuebingen.de>
</commit_message>
<xml_diff>
--- a/user-interface/src/main/resources/templates/ngs_measurement_registration_sheet.xlsx
+++ b/user-interface/src/main/resources/templates/ngs_measurement_registration_sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sven1103/git/data-manager/user-interface/src/main/resources/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/afriedrich/git/data-manager-app/user-interface/src/main/resources/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95CEBC0B-66F3-B142-A89B-9CF57FB4E8AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44060A07-D260-904A-9ABB-310DB2F9189F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{D4F19D33-EE39-EF46-8DDD-2818EAD74D6D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{D4F19D33-EE39-EF46-8DDD-2818EAD74D6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="96">
   <si>
     <t>facility</t>
   </si>
@@ -325,6 +325,9 @@
   </si>
   <si>
     <t>index i7</t>
+  </si>
+  <si>
+    <t>QBIC sample ids</t>
   </si>
 </sst>
 </file>
@@ -995,9 +998,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CA9A15C-9427-F34B-B818-4D616E8AFF0A}">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1015,7 +1016,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>2</v>
+        <v>95</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Remove sample codes from template
</commit_message>
<xml_diff>
--- a/user-interface/src/main/resources/templates/ngs_measurement_registration_sheet.xlsx
+++ b/user-interface/src/main/resources/templates/ngs_measurement_registration_sheet.xlsx
@@ -1,28 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steff\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE26E03C-D609-4D69-9323-12717A6CE5DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Metadata" sheetId="1" r:id="rId1"/>
-    <sheet name="Property information" sheetId="2" r:id="rId2"/>
-    <sheet name="Allowed-Values" sheetId="3" r:id="rId3"/>
+    <sheet name="Metadata" sheetId="1" r:id="rId4"/>
+    <sheet name="Property information" sheetId="2" r:id="rId5"/>
+    <sheet name="Allowed-Values" sheetId="3" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="49">
   <si>
     <t>QBIC sample ids*</t>
   </si>
@@ -63,21 +54,6 @@
     <t>Comment</t>
   </si>
   <si>
-    <t>Q007V001AM</t>
-  </si>
-  <si>
-    <t>Q007V002AU</t>
-  </si>
-  <si>
-    <t>Q007V004AC</t>
-  </si>
-  <si>
-    <t>Q007V003A4</t>
-  </si>
-  <si>
-    <t>Q007V005AK</t>
-  </si>
-  <si>
     <t>Measurement Property</t>
   </si>
   <si>
@@ -87,7 +63,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>QBIC sample id</t>
+    <t>QBIC sample ids</t>
   </si>
   <si>
     <t>mandatory</t>
@@ -135,16 +111,13 @@
     <t>Information on how many cycles for each read and index</t>
   </si>
   <si>
-    <t>In case of pooled sample get measuremed, indicate with a common sample group label for samples that are in the same measurement. Entries that share the same pool label will be combined as one measurement</t>
+    <t>In case of pooled sample get measured, indicate with a common sample group label for samples that are in the same measurement. Entries that share the same pool label will be combined as one measurement</t>
   </si>
   <si>
     <t>Index used for multiplexing</t>
   </si>
   <si>
     <t>Commenting notes about the measurement</t>
-  </si>
-  <si>
-    <t>QBIC sample id*</t>
   </si>
   <si>
     <t>one QBiC sample Id</t>
@@ -192,15 +165,28 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="0" formatCode="General"/>
+  </numFmts>
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Aptos Narrow"/>
     </font>
     <font>
-      <b/>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="1"/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
@@ -211,7 +197,7 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Arial"/>
@@ -306,29 +292,71 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+  <cellXfs count="20">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -337,85 +365,25 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFAAAAAA"/>
-      <rgbColor rgb="FFA7A7A7"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
+      <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffff0000"/>
+      <rgbColor rgb="ff00ff00"/>
+      <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="ffffff00"/>
+      <rgbColor rgb="ffff00ff"/>
+      <rgbColor rgb="ff00ffff"/>
+      <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ffa7a7a7"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -617,7 +585,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -635,7 +603,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -664,7 +632,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -689,7 +657,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -714,7 +682,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -739,7 +707,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -764,7 +732,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -789,7 +757,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -814,7 +782,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -839,7 +807,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -864,7 +832,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -877,15 +845,9 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -902,7 +864,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -920,7 +882,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -945,7 +907,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -970,7 +932,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -995,7 +957,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1020,7 +982,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1045,7 +1007,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1070,7 +1032,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1095,7 +1057,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1120,7 +1082,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1145,7 +1107,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1158,15 +1120,9 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1180,7 +1136,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1198,7 +1154,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1227,7 +1183,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1252,7 +1208,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1277,7 +1233,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1302,7 +1258,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1327,7 +1283,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1352,7 +1308,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1377,7 +1333,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1402,7 +1358,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1427,7 +1383,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1440,91 +1396,79 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.8333" defaultRowHeight="15.95" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="29.125" style="1" customWidth="1"/>
-    <col min="2" max="3" width="23.625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="29.1719" style="1" customWidth="1"/>
+    <col min="2" max="3" width="23.6719" style="1" customWidth="1"/>
     <col min="4" max="4" width="20.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.8516" style="1" customWidth="1"/>
     <col min="6" max="6" width="22.5" style="1" customWidth="1"/>
-    <col min="7" max="8" width="10.875" style="1" customWidth="1"/>
+    <col min="7" max="8" width="10.8516" style="1" customWidth="1"/>
     <col min="9" max="10" width="26" style="1" customWidth="1"/>
-    <col min="11" max="12" width="10.875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="101.375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="10.875" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="10.875" style="1"/>
+    <col min="11" max="12" width="10.8516" style="1" customWidth="1"/>
+    <col min="13" max="13" width="101.352" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="10.8516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" ht="13.5" customHeight="1">
+      <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s" s="2">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s" s="2">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s" s="2">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" t="s" s="2">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" t="s" s="2">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" t="s" s="2">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" t="s" s="2">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" t="s" s="2">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" t="s" s="2">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" t="s" s="2">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" t="s" s="2">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" t="s" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>13</v>
-      </c>
+    <row r="2" ht="17.1" customHeight="1">
+      <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -1538,10 +1482,8 @@
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
     </row>
-    <row r="3" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>14</v>
-      </c>
+    <row r="3" ht="17.1" customHeight="1">
+      <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -1555,10 +1497,8 @@
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>15</v>
-      </c>
+    <row r="4" ht="17.1" customHeight="1">
+      <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -1572,10 +1512,8 @@
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
     </row>
-    <row r="5" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>16</v>
-      </c>
+    <row r="5" ht="17.1" customHeight="1">
+      <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -1589,10 +1527,8 @@
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
     </row>
-    <row r="6" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>17</v>
-      </c>
+    <row r="6" ht="17.1" customHeight="1">
+      <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -1606,7 +1542,7 @@
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
     </row>
-    <row r="7" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" ht="17.1" customHeight="1">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -1621,7 +1557,7 @@
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
     </row>
-    <row r="8" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" ht="17.1" customHeight="1">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -1636,7 +1572,7 @@
       <c r="L8" s="8"/>
       <c r="M8" s="8"/>
     </row>
-    <row r="9" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" ht="17.1" customHeight="1">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -1651,7 +1587,7 @@
       <c r="L9" s="8"/>
       <c r="M9" s="8"/>
     </row>
-    <row r="10" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" ht="17.1" customHeight="1">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -1668,12 +1604,12 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F7:F10" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F7:F10">
       <formula1>"single-end,paired-end"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -1681,204 +1617,204 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.8333" defaultRowHeight="15.95" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="2" width="21.125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="86.125" style="1" customWidth="1"/>
-    <col min="4" max="6" width="10.875" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.875" style="1"/>
+    <col min="1" max="2" width="21.1719" style="11" customWidth="1"/>
+    <col min="3" max="3" width="86.1719" style="11" customWidth="1"/>
+    <col min="4" max="5" width="10.8516" style="11" customWidth="1"/>
+    <col min="6" max="16384" width="10.8516" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>20</v>
+    <row r="1" ht="17.1" customHeight="1">
+      <c r="A1" t="s" s="12">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s" s="12">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s" s="12">
+        <v>15</v>
       </c>
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
     </row>
-    <row r="2" spans="1:5" ht="26.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>23</v>
+    <row r="2" ht="26.65" customHeight="1">
+      <c r="A2" t="s" s="13">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s" s="13">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s" s="14">
+        <v>18</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" spans="1:5" ht="26.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+    <row r="3" ht="26.65" customHeight="1">
+      <c r="A3" t="s" s="13">
         <v>1</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>25</v>
+      <c r="B3" t="s" s="13">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s" s="14">
+        <v>20</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
     </row>
-    <row r="4" spans="1:5" ht="26.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="12" t="s">
+    <row r="4" ht="26.65" customHeight="1">
+      <c r="A4" t="s" s="13">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s" s="13">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s" s="14">
         <v>22</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>27</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>29</v>
+    <row r="5" ht="17.1" customHeight="1">
+      <c r="A5" t="s" s="13">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s" s="13">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s" s="14">
+        <v>24</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
     </row>
-    <row r="6" spans="1:5" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>31</v>
+    <row r="6" ht="39.6" customHeight="1">
+      <c r="A6" t="s" s="13">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s" s="13">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s" s="14">
+        <v>26</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
     </row>
-    <row r="7" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>33</v>
+    <row r="7" ht="17.1" customHeight="1">
+      <c r="A7" t="s" s="13">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s" s="13">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s" s="14">
+        <v>28</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
     </row>
-    <row r="8" spans="1:5" ht="26.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+    <row r="8" ht="26.65" customHeight="1">
+      <c r="A8" t="s" s="13">
         <v>6</v>
       </c>
-      <c r="B8" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>34</v>
+      <c r="B8" t="s" s="13">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s" s="14">
+        <v>29</v>
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
     </row>
-    <row r="9" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+    <row r="9" ht="17.1" customHeight="1">
+      <c r="A9" t="s" s="13">
         <v>7</v>
       </c>
-      <c r="B9" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>35</v>
+      <c r="B9" t="s" s="13">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s" s="14">
+        <v>30</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
     </row>
-    <row r="10" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+    <row r="10" ht="17.1" customHeight="1">
+      <c r="A10" t="s" s="13">
         <v>8</v>
       </c>
-      <c r="B10" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>36</v>
+      <c r="B10" t="s" s="13">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s" s="14">
+        <v>31</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
     </row>
-    <row r="11" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
+    <row r="11" ht="17.1" customHeight="1">
+      <c r="A11" t="s" s="13">
         <v>9</v>
       </c>
-      <c r="B11" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>37</v>
+      <c r="B11" t="s" s="13">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s" s="14">
+        <v>32</v>
       </c>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
     </row>
-    <row r="12" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
+    <row r="12" ht="17.1" customHeight="1">
+      <c r="A12" t="s" s="13">
         <v>10</v>
       </c>
-      <c r="B12" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>38</v>
+      <c r="B12" t="s" s="14">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s" s="14">
+        <v>33</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
     </row>
-    <row r="13" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
+    <row r="13" ht="17.1" customHeight="1">
+      <c r="A13" t="s" s="13">
         <v>11</v>
       </c>
-      <c r="B13" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>38</v>
+      <c r="B13" t="s" s="14">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s" s="14">
+        <v>33</v>
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
     </row>
-    <row r="14" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="12" t="s">
+    <row r="14" ht="17.1" customHeight="1">
+      <c r="A14" t="s" s="13">
         <v>12</v>
       </c>
-      <c r="B14" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>39</v>
+      <c r="B14" t="s" s="13">
+        <v>19</v>
+      </c>
+      <c r="C14" t="s" s="14">
+        <v>34</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -1886,142 +1822,139 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.8333" defaultRowHeight="15.95" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="30.375" style="1" customWidth="1"/>
-    <col min="2" max="3" width="16" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="35.875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="26.625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="22.875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="19.125" style="1" customWidth="1"/>
-    <col min="11" max="12" width="16.625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="24" style="1" customWidth="1"/>
-    <col min="14" max="14" width="10.875" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="10.875" style="1"/>
+    <col min="1" max="1" width="30.3516" style="15" customWidth="1"/>
+    <col min="2" max="3" width="16" style="15" customWidth="1"/>
+    <col min="4" max="4" width="18.6719" style="15" customWidth="1"/>
+    <col min="5" max="5" width="35.8516" style="15" customWidth="1"/>
+    <col min="6" max="6" width="26.6719" style="15" customWidth="1"/>
+    <col min="7" max="7" width="15.3516" style="15" customWidth="1"/>
+    <col min="8" max="8" width="14.8516" style="15" customWidth="1"/>
+    <col min="9" max="9" width="22.8516" style="15" customWidth="1"/>
+    <col min="10" max="10" width="19.1719" style="15" customWidth="1"/>
+    <col min="11" max="12" width="16.6719" style="15" customWidth="1"/>
+    <col min="13" max="13" width="24" style="15" customWidth="1"/>
+    <col min="14" max="16384" width="10.8516" style="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" ht="13.5" customHeight="1">
+      <c r="A1" t="s" s="16">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="16">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s" s="16">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s" s="16">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s" s="16">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s" s="16">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s" s="16">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s" s="16">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s" s="16">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s" s="16">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s" s="16">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s" s="16">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s" s="16">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" ht="13.5" customHeight="1">
+      <c r="A2" t="s" s="13">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s" s="13">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s" s="13">
+        <v>37</v>
+      </c>
+      <c r="D2" t="s" s="13">
+        <v>38</v>
+      </c>
+      <c r="E2" t="s" s="13">
+        <v>39</v>
+      </c>
+      <c r="F2" t="s" s="13">
         <v>40</v>
       </c>
-      <c r="B1" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="G2" t="s" s="13">
+        <v>36</v>
+      </c>
+      <c r="H2" t="s" s="13">
+        <v>36</v>
+      </c>
+      <c r="I2" t="s" s="13">
+        <v>36</v>
+      </c>
+      <c r="J2" t="s" s="17">
         <v>41</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="K2" t="s" s="13">
+        <v>36</v>
+      </c>
+      <c r="L2" t="s" s="13">
+        <v>36</v>
+      </c>
+      <c r="M2" t="s" s="13">
         <v>42</v>
       </c>
-      <c r="C2" s="12" t="s">
+    </row>
+    <row r="3" ht="13.5" customHeight="1">
+      <c r="A3" t="s" s="13">
         <v>43</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="B3" s="13"/>
+      <c r="C3" t="s" s="13">
         <v>44</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="D3" s="10"/>
+      <c r="E3" t="s" s="13">
         <v>45</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F3" t="s" s="13">
         <v>46</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="J2" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="L2" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="M2" s="12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>52</v>
       </c>
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
-      <c r="J3" s="12"/>
+      <c r="J3" s="13"/>
       <c r="K3" s="10"/>
       <c r="L3" s="10"/>
       <c r="M3" s="10"/>
     </row>
-    <row r="4" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="10"/>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
-      <c r="E4" s="12" t="s">
-        <v>53</v>
+      <c r="E4" t="s" s="13">
+        <v>47</v>
       </c>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
@@ -2030,15 +1963,15 @@
       <c r="J4" s="10"/>
       <c r="K4" s="10"/>
       <c r="L4" s="10"/>
-      <c r="M4" s="16"/>
-    </row>
-    <row r="5" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M4" s="18"/>
+    </row>
+    <row r="5" ht="13.5" customHeight="1">
       <c r="A5" s="10"/>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
-      <c r="E5" s="12" t="s">
-        <v>54</v>
+      <c r="E5" t="s" s="13">
+        <v>48</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
@@ -2049,7 +1982,7 @@
       <c r="L5" s="10"/>
       <c r="M5" s="10"/>
     </row>
-    <row r="6" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" ht="13.5" customHeight="1">
       <c r="A6" s="10"/>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
@@ -2064,7 +1997,7 @@
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
     </row>
-    <row r="7" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" ht="13.5" customHeight="1">
       <c r="A7" s="10"/>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
@@ -2079,7 +2012,7 @@
       <c r="L7" s="10"/>
       <c r="M7" s="10"/>
     </row>
-    <row r="8" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" ht="13.5" customHeight="1">
       <c r="A8" s="10"/>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
@@ -2094,7 +2027,7 @@
       <c r="L8" s="10"/>
       <c r="M8" s="10"/>
     </row>
-    <row r="9" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" ht="13.5" customHeight="1">
       <c r="A9" s="10"/>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
@@ -2109,7 +2042,7 @@
       <c r="L9" s="10"/>
       <c r="M9" s="10"/>
     </row>
-    <row r="10" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" ht="13.5" customHeight="1">
       <c r="A10" s="10"/>
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
@@ -2124,7 +2057,7 @@
       <c r="L10" s="10"/>
       <c r="M10" s="10"/>
     </row>
-    <row r="11" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" ht="13.5" customHeight="1">
       <c r="A11" s="10"/>
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
@@ -2139,7 +2072,7 @@
       <c r="L11" s="10"/>
       <c r="M11" s="10"/>
     </row>
-    <row r="12" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" ht="13.5" customHeight="1">
       <c r="A12" s="10"/>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
@@ -2154,7 +2087,7 @@
       <c r="L12" s="10"/>
       <c r="M12" s="10"/>
     </row>
-    <row r="13" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" ht="13.5" customHeight="1">
       <c r="A13" s="10"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
@@ -2169,7 +2102,7 @@
       <c r="L13" s="10"/>
       <c r="M13" s="10"/>
     </row>
-    <row r="14" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" ht="13.5" customHeight="1">
       <c r="A14" s="10"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
@@ -2184,7 +2117,7 @@
       <c r="L14" s="10"/>
       <c r="M14" s="10"/>
     </row>
-    <row r="15" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" ht="13.5" customHeight="1">
       <c r="A15" s="10"/>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
@@ -2199,7 +2132,7 @@
       <c r="L15" s="10"/>
       <c r="M15" s="10"/>
     </row>
-    <row r="16" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" ht="13.5" customHeight="1">
       <c r="A16" s="10"/>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
@@ -2214,7 +2147,7 @@
       <c r="L16" s="10"/>
       <c r="M16" s="10"/>
     </row>
-    <row r="17" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" ht="13.5" customHeight="1">
       <c r="A17" s="10"/>
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
@@ -2229,7 +2162,7 @@
       <c r="L17" s="10"/>
       <c r="M17" s="10"/>
     </row>
-    <row r="18" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" ht="13.5" customHeight="1">
       <c r="A18" s="10"/>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
@@ -2244,84 +2177,84 @@
       <c r="L18" s="10"/>
       <c r="M18" s="10"/>
     </row>
-    <row r="19" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="17"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="17"/>
-      <c r="K19" s="17"/>
-      <c r="L19" s="17"/>
-      <c r="M19" s="17"/>
-    </row>
-    <row r="20" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="17"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="17"/>
-      <c r="J20" s="17"/>
-      <c r="K20" s="17"/>
-      <c r="L20" s="17"/>
-      <c r="M20" s="17"/>
-    </row>
-    <row r="21" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="17"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="17"/>
-      <c r="K21" s="17"/>
-      <c r="L21" s="17"/>
-      <c r="M21" s="17"/>
-    </row>
-    <row r="22" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="17"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17"/>
-      <c r="K22" s="17"/>
-      <c r="L22" s="17"/>
-      <c r="M22" s="17"/>
-    </row>
-    <row r="23" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="17"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="17"/>
-      <c r="K23" s="17"/>
-      <c r="L23" s="17"/>
-      <c r="M23" s="17"/>
+    <row r="19" ht="15.95" customHeight="1">
+      <c r="A19" s="19"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="19"/>
+      <c r="L19" s="19"/>
+      <c r="M19" s="19"/>
+    </row>
+    <row r="20" ht="15.95" customHeight="1">
+      <c r="A20" s="19"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="19"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="19"/>
+      <c r="M20" s="19"/>
+    </row>
+    <row r="21" ht="15.95" customHeight="1">
+      <c r="A21" s="19"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="19"/>
+      <c r="L21" s="19"/>
+      <c r="M21" s="19"/>
+    </row>
+    <row r="22" ht="15.95" customHeight="1">
+      <c r="A22" s="19"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="19"/>
+      <c r="K22" s="19"/>
+      <c r="L22" s="19"/>
+      <c r="M22" s="19"/>
+    </row>
+    <row r="23" ht="15.95" customHeight="1">
+      <c r="A23" s="19"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="19"/>
+      <c r="L23" s="19"/>
+      <c r="M23" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Fix typo and naming description in columns of template sheets
</commit_message>
<xml_diff>
--- a/user-interface/src/main/resources/templates/ngs_measurement_registration_sheet.xlsx
+++ b/user-interface/src/main/resources/templates/ngs_measurement_registration_sheet.xlsx
@@ -13,9 +13,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="49">
-  <si>
-    <t>QBIC sample ids*</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="47">
+  <si>
+    <t>QBIC sample id*</t>
   </si>
   <si>
     <t>Sample Label</t>
@@ -63,13 +63,13 @@
     <t>Description</t>
   </si>
   <si>
-    <t>QBIC sample ids</t>
+    <t>QBIC sample id</t>
   </si>
   <si>
     <t>mandatory</t>
   </si>
   <si>
-    <t>Each measurement need to be linked to at least on analyte sample. You can provide more than one sample id in case you have non demultiplexed samples. Just provide the ids  ',' (comma) separated</t>
+    <t>Each measurement need to be linked to at least on analyte sample.</t>
   </si>
   <si>
     <t>optional</t>
@@ -135,9 +135,6 @@
     <t xml:space="preserve">ontology CURIE (e.g. EFO:0008637) </t>
   </si>
   <si>
-    <t>single-end</t>
-  </si>
-  <si>
     <t>number (e.g. 1, 2, 3)</t>
   </si>
   <si>
@@ -151,9 +148,6 @@
   </si>
   <si>
     <t>Currently supported ontologies:</t>
-  </si>
-  <si>
-    <t>paired-end</t>
   </si>
   <si>
     <t>https://www.ebi.ac.uk/ols4/ontologies/efo</t>
@@ -296,7 +290,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -348,7 +342,10 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1844,102 +1841,100 @@
   </cols>
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
-      <c r="A1" t="s" s="16">
+      <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="16">
+      <c r="B1" t="s" s="2">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="16">
+      <c r="C1" t="s" s="2">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="16">
+      <c r="D1" t="s" s="2">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="16">
+      <c r="E1" t="s" s="2">
         <v>4</v>
       </c>
       <c r="F1" t="s" s="16">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="16">
+      <c r="G1" t="s" s="2">
         <v>6</v>
       </c>
-      <c r="H1" t="s" s="16">
+      <c r="H1" t="s" s="2">
         <v>7</v>
       </c>
-      <c r="I1" t="s" s="16">
+      <c r="I1" t="s" s="2">
         <v>8</v>
       </c>
-      <c r="J1" t="s" s="16">
+      <c r="J1" t="s" s="2">
         <v>9</v>
       </c>
-      <c r="K1" t="s" s="16">
+      <c r="K1" t="s" s="2">
         <v>10</v>
       </c>
-      <c r="L1" t="s" s="16">
+      <c r="L1" t="s" s="2">
         <v>11</v>
       </c>
-      <c r="M1" t="s" s="16">
+      <c r="M1" t="s" s="2">
         <v>12</v>
       </c>
     </row>
     <row r="2" ht="13.5" customHeight="1">
-      <c r="A2" t="s" s="13">
+      <c r="A2" t="s" s="17">
         <v>35</v>
       </c>
-      <c r="B2" t="s" s="13">
+      <c r="B2" t="s" s="17">
         <v>36</v>
       </c>
-      <c r="C2" t="s" s="13">
+      <c r="C2" t="s" s="17">
         <v>37</v>
       </c>
-      <c r="D2" t="s" s="13">
+      <c r="D2" t="s" s="17">
         <v>38</v>
       </c>
-      <c r="E2" t="s" s="13">
+      <c r="E2" t="s" s="17">
         <v>39</v>
       </c>
       <c r="F2" t="s" s="13">
+        <v>36</v>
+      </c>
+      <c r="G2" t="s" s="17">
+        <v>36</v>
+      </c>
+      <c r="H2" t="s" s="17">
+        <v>36</v>
+      </c>
+      <c r="I2" t="s" s="17">
+        <v>36</v>
+      </c>
+      <c r="J2" t="s" s="18">
         <v>40</v>
       </c>
-      <c r="G2" t="s" s="13">
+      <c r="K2" t="s" s="17">
         <v>36</v>
       </c>
-      <c r="H2" t="s" s="13">
+      <c r="L2" t="s" s="17">
         <v>36</v>
       </c>
-      <c r="I2" t="s" s="13">
-        <v>36</v>
-      </c>
-      <c r="J2" t="s" s="17">
+      <c r="M2" t="s" s="17">
         <v>41</v>
-      </c>
-      <c r="K2" t="s" s="13">
-        <v>36</v>
-      </c>
-      <c r="L2" t="s" s="13">
-        <v>36</v>
-      </c>
-      <c r="M2" t="s" s="13">
-        <v>42</v>
       </c>
     </row>
     <row r="3" ht="13.5" customHeight="1">
       <c r="A3" t="s" s="13">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" s="13"/>
       <c r="C3" t="s" s="13">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" t="s" s="13">
-        <v>45</v>
-      </c>
-      <c r="F3" t="s" s="13">
-        <v>46</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="F3" s="13"/>
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
@@ -1954,7 +1949,7 @@
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
       <c r="E4" t="s" s="13">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
@@ -1963,7 +1958,7 @@
       <c r="J4" s="10"/>
       <c r="K4" s="10"/>
       <c r="L4" s="10"/>
-      <c r="M4" s="18"/>
+      <c r="M4" s="19"/>
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="A5" s="10"/>
@@ -1971,7 +1966,7 @@
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
       <c r="E5" t="s" s="13">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
@@ -2178,79 +2173,79 @@
       <c r="M18" s="10"/>
     </row>
     <row r="19" ht="15.95" customHeight="1">
-      <c r="A19" s="19"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="19"/>
-      <c r="K19" s="19"/>
-      <c r="L19" s="19"/>
-      <c r="M19" s="19"/>
+      <c r="A19" s="20"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
+      <c r="M19" s="20"/>
     </row>
     <row r="20" ht="15.95" customHeight="1">
-      <c r="A20" s="19"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="19"/>
-      <c r="K20" s="19"/>
-      <c r="L20" s="19"/>
-      <c r="M20" s="19"/>
+      <c r="A20" s="20"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="20"/>
+      <c r="L20" s="20"/>
+      <c r="M20" s="20"/>
     </row>
     <row r="21" ht="15.95" customHeight="1">
-      <c r="A21" s="19"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="19"/>
-      <c r="J21" s="19"/>
-      <c r="K21" s="19"/>
-      <c r="L21" s="19"/>
-      <c r="M21" s="19"/>
+      <c r="A21" s="20"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="20"/>
+      <c r="L21" s="20"/>
+      <c r="M21" s="20"/>
     </row>
     <row r="22" ht="15.95" customHeight="1">
-      <c r="A22" s="19"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
-      <c r="J22" s="19"/>
-      <c r="K22" s="19"/>
-      <c r="L22" s="19"/>
-      <c r="M22" s="19"/>
+      <c r="A22" s="20"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="20"/>
+      <c r="L22" s="20"/>
+      <c r="M22" s="20"/>
     </row>
     <row r="23" ht="15.95" customHeight="1">
-      <c r="A23" s="19"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="19"/>
-      <c r="J23" s="19"/>
-      <c r="K23" s="19"/>
-      <c r="L23" s="19"/>
-      <c r="M23" s="19"/>
+      <c r="A23" s="20"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="20"/>
+      <c r="L23" s="20"/>
+      <c r="M23" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix typo and naming description in columns of template sheets (#541)
</commit_message>
<xml_diff>
--- a/user-interface/src/main/resources/templates/ngs_measurement_registration_sheet.xlsx
+++ b/user-interface/src/main/resources/templates/ngs_measurement_registration_sheet.xlsx
@@ -13,9 +13,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="49">
-  <si>
-    <t>QBIC sample ids*</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="47">
+  <si>
+    <t>QBIC sample id*</t>
   </si>
   <si>
     <t>Sample Label</t>
@@ -63,13 +63,13 @@
     <t>Description</t>
   </si>
   <si>
-    <t>QBIC sample ids</t>
+    <t>QBIC sample id</t>
   </si>
   <si>
     <t>mandatory</t>
   </si>
   <si>
-    <t>Each measurement need to be linked to at least on analyte sample. You can provide more than one sample id in case you have non demultiplexed samples. Just provide the ids  ',' (comma) separated</t>
+    <t>Each measurement need to be linked to at least on analyte sample.</t>
   </si>
   <si>
     <t>optional</t>
@@ -135,9 +135,6 @@
     <t xml:space="preserve">ontology CURIE (e.g. EFO:0008637) </t>
   </si>
   <si>
-    <t>single-end</t>
-  </si>
-  <si>
     <t>number (e.g. 1, 2, 3)</t>
   </si>
   <si>
@@ -151,9 +148,6 @@
   </si>
   <si>
     <t>Currently supported ontologies:</t>
-  </si>
-  <si>
-    <t>paired-end</t>
   </si>
   <si>
     <t>https://www.ebi.ac.uk/ols4/ontologies/efo</t>
@@ -296,7 +290,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -348,7 +342,10 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1844,102 +1841,100 @@
   </cols>
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
-      <c r="A1" t="s" s="16">
+      <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="16">
+      <c r="B1" t="s" s="2">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="16">
+      <c r="C1" t="s" s="2">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="16">
+      <c r="D1" t="s" s="2">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="16">
+      <c r="E1" t="s" s="2">
         <v>4</v>
       </c>
       <c r="F1" t="s" s="16">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="16">
+      <c r="G1" t="s" s="2">
         <v>6</v>
       </c>
-      <c r="H1" t="s" s="16">
+      <c r="H1" t="s" s="2">
         <v>7</v>
       </c>
-      <c r="I1" t="s" s="16">
+      <c r="I1" t="s" s="2">
         <v>8</v>
       </c>
-      <c r="J1" t="s" s="16">
+      <c r="J1" t="s" s="2">
         <v>9</v>
       </c>
-      <c r="K1" t="s" s="16">
+      <c r="K1" t="s" s="2">
         <v>10</v>
       </c>
-      <c r="L1" t="s" s="16">
+      <c r="L1" t="s" s="2">
         <v>11</v>
       </c>
-      <c r="M1" t="s" s="16">
+      <c r="M1" t="s" s="2">
         <v>12</v>
       </c>
     </row>
     <row r="2" ht="13.5" customHeight="1">
-      <c r="A2" t="s" s="13">
+      <c r="A2" t="s" s="17">
         <v>35</v>
       </c>
-      <c r="B2" t="s" s="13">
+      <c r="B2" t="s" s="17">
         <v>36</v>
       </c>
-      <c r="C2" t="s" s="13">
+      <c r="C2" t="s" s="17">
         <v>37</v>
       </c>
-      <c r="D2" t="s" s="13">
+      <c r="D2" t="s" s="17">
         <v>38</v>
       </c>
-      <c r="E2" t="s" s="13">
+      <c r="E2" t="s" s="17">
         <v>39</v>
       </c>
       <c r="F2" t="s" s="13">
+        <v>36</v>
+      </c>
+      <c r="G2" t="s" s="17">
+        <v>36</v>
+      </c>
+      <c r="H2" t="s" s="17">
+        <v>36</v>
+      </c>
+      <c r="I2" t="s" s="17">
+        <v>36</v>
+      </c>
+      <c r="J2" t="s" s="18">
         <v>40</v>
       </c>
-      <c r="G2" t="s" s="13">
+      <c r="K2" t="s" s="17">
         <v>36</v>
       </c>
-      <c r="H2" t="s" s="13">
+      <c r="L2" t="s" s="17">
         <v>36</v>
       </c>
-      <c r="I2" t="s" s="13">
-        <v>36</v>
-      </c>
-      <c r="J2" t="s" s="17">
+      <c r="M2" t="s" s="17">
         <v>41</v>
-      </c>
-      <c r="K2" t="s" s="13">
-        <v>36</v>
-      </c>
-      <c r="L2" t="s" s="13">
-        <v>36</v>
-      </c>
-      <c r="M2" t="s" s="13">
-        <v>42</v>
       </c>
     </row>
     <row r="3" ht="13.5" customHeight="1">
       <c r="A3" t="s" s="13">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" s="13"/>
       <c r="C3" t="s" s="13">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" t="s" s="13">
-        <v>45</v>
-      </c>
-      <c r="F3" t="s" s="13">
-        <v>46</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="F3" s="13"/>
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
@@ -1954,7 +1949,7 @@
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
       <c r="E4" t="s" s="13">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
@@ -1963,7 +1958,7 @@
       <c r="J4" s="10"/>
       <c r="K4" s="10"/>
       <c r="L4" s="10"/>
-      <c r="M4" s="18"/>
+      <c r="M4" s="19"/>
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="A5" s="10"/>
@@ -1971,7 +1966,7 @@
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
       <c r="E5" t="s" s="13">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
@@ -2178,79 +2173,79 @@
       <c r="M18" s="10"/>
     </row>
     <row r="19" ht="15.95" customHeight="1">
-      <c r="A19" s="19"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="19"/>
-      <c r="K19" s="19"/>
-      <c r="L19" s="19"/>
-      <c r="M19" s="19"/>
+      <c r="A19" s="20"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
+      <c r="M19" s="20"/>
     </row>
     <row r="20" ht="15.95" customHeight="1">
-      <c r="A20" s="19"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="19"/>
-      <c r="K20" s="19"/>
-      <c r="L20" s="19"/>
-      <c r="M20" s="19"/>
+      <c r="A20" s="20"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="20"/>
+      <c r="L20" s="20"/>
+      <c r="M20" s="20"/>
     </row>
     <row r="21" ht="15.95" customHeight="1">
-      <c r="A21" s="19"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="19"/>
-      <c r="J21" s="19"/>
-      <c r="K21" s="19"/>
-      <c r="L21" s="19"/>
-      <c r="M21" s="19"/>
+      <c r="A21" s="20"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="20"/>
+      <c r="L21" s="20"/>
+      <c r="M21" s="20"/>
     </row>
     <row r="22" ht="15.95" customHeight="1">
-      <c r="A22" s="19"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
-      <c r="J22" s="19"/>
-      <c r="K22" s="19"/>
-      <c r="L22" s="19"/>
-      <c r="M22" s="19"/>
+      <c r="A22" s="20"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="20"/>
+      <c r="L22" s="20"/>
+      <c r="M22" s="20"/>
     </row>
     <row r="23" ht="15.95" customHeight="1">
-      <c r="A23" s="19"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="19"/>
-      <c r="J23" s="19"/>
-      <c r="K23" s="19"/>
-      <c r="L23" s="19"/>
-      <c r="M23" s="19"/>
+      <c r="A23" s="20"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="20"/>
+      <c r="L23" s="20"/>
+      <c r="M23" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix pooling for registration and move pooling group to beginning of ngs template
</commit_message>
<xml_diff>
--- a/user-interface/src/main/resources/templates/ngs_measurement_registration_sheet.xlsx
+++ b/user-interface/src/main/resources/templates/ngs_measurement_registration_sheet.xlsx
@@ -21,6 +21,9 @@
     <t>Sample Label</t>
   </si>
   <si>
+    <t>Sample Pool Group</t>
+  </si>
+  <si>
     <t>Organisation id*</t>
   </si>
   <si>
@@ -42,9 +45,6 @@
     <t>Sequencing run protocol</t>
   </si>
   <si>
-    <t>Sample Pool Group</t>
-  </si>
-  <si>
     <t>Index i7</t>
   </si>
   <si>
@@ -78,6 +78,9 @@
     <t>This is just a visual aid simplify sample navigation. This column gets ignored during measurement registration</t>
   </si>
   <si>
+    <t>In case of pooled sample get measured, indicate with a common sample group label for samples that are in the same measurement. Entries that share the same pool label will be combined as one measurement</t>
+  </si>
+  <si>
     <t>Organisation id</t>
   </si>
   <si>
@@ -111,9 +114,6 @@
     <t>Information on how many cycles for each read and index</t>
   </si>
   <si>
-    <t>In case of pooled sample get measured, indicate with a common sample group label for samples that are in the same measurement. Entries that share the same pool label will be combined as one measurement</t>
-  </si>
-  <si>
     <t>Index used for multiplexing</t>
   </si>
   <si>
@@ -126,6 +126,9 @@
     <t>Free text</t>
   </si>
   <si>
+    <t>number (e.g. 1, 2, 3)</t>
+  </si>
+  <si>
     <t>full ROR url</t>
   </si>
   <si>
@@ -133,9 +136,6 @@
   </si>
   <si>
     <t xml:space="preserve">ontology CURIE (e.g. EFO:0008637) </t>
-  </si>
-  <si>
-    <t>number (e.g. 1, 2, 3)</t>
   </si>
   <si>
     <t>free text (max. 500 characters)</t>
@@ -309,19 +309,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -1412,12 +1412,14 @@
   <sheetFormatPr defaultColWidth="10.8333" defaultRowHeight="15.95" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="29.1719" style="1" customWidth="1"/>
-    <col min="2" max="3" width="23.6719" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.8516" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.5" style="1" customWidth="1"/>
-    <col min="7" max="8" width="10.8516" style="1" customWidth="1"/>
-    <col min="9" max="10" width="26" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23.6719" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.6719" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.8516" style="1" customWidth="1"/>
+    <col min="7" max="7" width="22.5" style="1" customWidth="1"/>
+    <col min="8" max="9" width="10.8516" style="1" customWidth="1"/>
+    <col min="10" max="10" width="26" style="1" customWidth="1"/>
     <col min="11" max="12" width="10.8516" style="1" customWidth="1"/>
     <col min="13" max="13" width="101.352" style="1" customWidth="1"/>
     <col min="14" max="16384" width="10.8516" style="1" customWidth="1"/>
@@ -1467,14 +1469,14 @@
     <row r="2" ht="17.1" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
+      <c r="C2" s="4"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
-      <c r="J2" s="4"/>
+      <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
@@ -1482,14 +1484,14 @@
     <row r="3" ht="17.1" customHeight="1">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
+      <c r="C3" s="4"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
-      <c r="J3" s="4"/>
+      <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
@@ -1497,14 +1499,14 @@
     <row r="4" ht="17.1" customHeight="1">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
+      <c r="C4" s="4"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
-      <c r="J4" s="4"/>
+      <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
@@ -1512,14 +1514,14 @@
     <row r="5" ht="17.1" customHeight="1">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
+      <c r="C5" s="4"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
-      <c r="J5" s="4"/>
+      <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
@@ -1527,14 +1529,14 @@
     <row r="6" ht="17.1" customHeight="1">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
+      <c r="C6" s="4"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
-      <c r="J6" s="4"/>
+      <c r="J6" s="3"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
@@ -1542,14 +1544,14 @@
     <row r="7" ht="17.1" customHeight="1">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
+      <c r="C7" s="6"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="7"/>
       <c r="I7" s="5"/>
-      <c r="J7" s="7"/>
+      <c r="J7" s="5"/>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
@@ -1557,14 +1559,14 @@
     <row r="8" ht="17.1" customHeight="1">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
+      <c r="C8" s="9"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="10"/>
       <c r="I8" s="8"/>
-      <c r="J8" s="10"/>
+      <c r="J8" s="8"/>
       <c r="K8" s="8"/>
       <c r="L8" s="8"/>
       <c r="M8" s="8"/>
@@ -1572,14 +1574,14 @@
     <row r="9" ht="17.1" customHeight="1">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
+      <c r="C9" s="9"/>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="10"/>
       <c r="I9" s="8"/>
-      <c r="J9" s="10"/>
+      <c r="J9" s="8"/>
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
       <c r="M9" s="8"/>
@@ -1587,21 +1589,21 @@
     <row r="10" ht="17.1" customHeight="1">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
+      <c r="C10" s="9"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="10"/>
       <c r="I10" s="8"/>
-      <c r="J10" s="10"/>
+      <c r="J10" s="8"/>
       <c r="K10" s="8"/>
       <c r="L10" s="8"/>
       <c r="M10" s="8"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F7:F10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G7:G10">
       <formula1>"single-end,paired-end"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1666,64 +1668,64 @@
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
     </row>
-    <row r="4" ht="26.65" customHeight="1">
+    <row r="4" ht="17.1" customHeight="1">
       <c r="A4" t="s" s="13">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s" s="13">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s" s="14">
         <v>21</v>
-      </c>
-      <c r="B4" t="s" s="13">
-        <v>17</v>
-      </c>
-      <c r="C4" t="s" s="14">
-        <v>22</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" ht="17.1" customHeight="1">
+    <row r="5" ht="26.65" customHeight="1">
       <c r="A5" t="s" s="13">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s" s="13">
         <v>17</v>
       </c>
       <c r="C5" t="s" s="14">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
     </row>
-    <row r="6" ht="39.6" customHeight="1">
+    <row r="6" ht="17.1" customHeight="1">
       <c r="A6" t="s" s="13">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s" s="13">
         <v>17</v>
       </c>
       <c r="C6" t="s" s="14">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
     </row>
-    <row r="7" ht="17.1" customHeight="1">
+    <row r="7" ht="39.6" customHeight="1">
       <c r="A7" t="s" s="13">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s" s="13">
         <v>17</v>
       </c>
       <c r="C7" t="s" s="14">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
     </row>
-    <row r="8" ht="26.65" customHeight="1">
+    <row r="8" ht="17.1" customHeight="1">
       <c r="A8" t="s" s="13">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s" s="13">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s" s="14">
         <v>29</v>
@@ -1731,7 +1733,7 @@
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
     </row>
-    <row r="9" ht="17.1" customHeight="1">
+    <row r="9" ht="26.65" customHeight="1">
       <c r="A9" t="s" s="13">
         <v>7</v>
       </c>
@@ -1827,14 +1829,15 @@
   <sheetFormatPr defaultColWidth="10.8333" defaultRowHeight="15.95" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="30.3516" style="15" customWidth="1"/>
-    <col min="2" max="3" width="16" style="15" customWidth="1"/>
-    <col min="4" max="4" width="18.6719" style="15" customWidth="1"/>
-    <col min="5" max="5" width="35.8516" style="15" customWidth="1"/>
-    <col min="6" max="6" width="26.6719" style="15" customWidth="1"/>
-    <col min="7" max="7" width="15.3516" style="15" customWidth="1"/>
-    <col min="8" max="8" width="14.8516" style="15" customWidth="1"/>
-    <col min="9" max="9" width="22.8516" style="15" customWidth="1"/>
-    <col min="10" max="10" width="19.1719" style="15" customWidth="1"/>
+    <col min="2" max="2" width="16" style="15" customWidth="1"/>
+    <col min="3" max="3" width="19.1719" style="15" customWidth="1"/>
+    <col min="4" max="4" width="16" style="15" customWidth="1"/>
+    <col min="5" max="5" width="18.6719" style="15" customWidth="1"/>
+    <col min="6" max="6" width="35.8516" style="15" customWidth="1"/>
+    <col min="7" max="7" width="26.6719" style="15" customWidth="1"/>
+    <col min="8" max="8" width="15.3516" style="15" customWidth="1"/>
+    <col min="9" max="9" width="14.8516" style="15" customWidth="1"/>
+    <col min="10" max="10" width="22.8516" style="15" customWidth="1"/>
     <col min="11" max="12" width="16.6719" style="15" customWidth="1"/>
     <col min="13" max="13" width="24" style="15" customWidth="1"/>
     <col min="14" max="16384" width="10.8516" style="15" customWidth="1"/>
@@ -1856,10 +1859,10 @@
       <c r="E1" t="s" s="2">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="16">
+      <c r="F1" t="s" s="2">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="2">
+      <c r="G1" t="s" s="16">
         <v>6</v>
       </c>
       <c r="H1" t="s" s="2">
@@ -1888,7 +1891,7 @@
       <c r="B2" t="s" s="17">
         <v>36</v>
       </c>
-      <c r="C2" t="s" s="17">
+      <c r="C2" t="s" s="18">
         <v>37</v>
       </c>
       <c r="D2" t="s" s="17">
@@ -1897,10 +1900,10 @@
       <c r="E2" t="s" s="17">
         <v>39</v>
       </c>
-      <c r="F2" t="s" s="13">
-        <v>36</v>
-      </c>
-      <c r="G2" t="s" s="17">
+      <c r="F2" t="s" s="17">
+        <v>40</v>
+      </c>
+      <c r="G2" t="s" s="13">
         <v>36</v>
       </c>
       <c r="H2" t="s" s="17">
@@ -1909,8 +1912,8 @@
       <c r="I2" t="s" s="17">
         <v>36</v>
       </c>
-      <c r="J2" t="s" s="18">
-        <v>40</v>
+      <c r="J2" t="s" s="17">
+        <v>36</v>
       </c>
       <c r="K2" t="s" s="17">
         <v>36</v>
@@ -1927,250 +1930,250 @@
         <v>42</v>
       </c>
       <c r="B3" s="13"/>
-      <c r="C3" t="s" s="13">
+      <c r="C3" s="13"/>
+      <c r="D3" t="s" s="13">
         <v>43</v>
       </c>
-      <c r="D3" s="10"/>
-      <c r="E3" t="s" s="13">
+      <c r="E3" s="9"/>
+      <c r="F3" t="s" s="13">
         <v>44</v>
       </c>
-      <c r="F3" s="13"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
     </row>
     <row r="4" ht="13.5" customHeight="1">
-      <c r="A4" s="10"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" t="s" s="13">
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" t="s" s="13">
         <v>45</v>
       </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
       <c r="M4" s="19"/>
     </row>
     <row r="5" ht="13.5" customHeight="1">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" t="s" s="13">
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" t="s" s="13">
         <v>46</v>
       </c>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
     </row>
     <row r="6" ht="13.5" customHeight="1">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
     </row>
     <row r="7" ht="13.5" customHeight="1">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
     </row>
     <row r="8" ht="13.5" customHeight="1">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
     </row>
     <row r="9" ht="13.5" customHeight="1">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
     </row>
     <row r="10" ht="13.5" customHeight="1">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
     </row>
     <row r="11" ht="13.5" customHeight="1">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
     </row>
     <row r="12" ht="13.5" customHeight="1">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
     </row>
     <row r="13" ht="13.5" customHeight="1">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
     </row>
     <row r="14" ht="13.5" customHeight="1">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
     </row>
     <row r="15" ht="13.5" customHeight="1">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
     </row>
     <row r="16" ht="13.5" customHeight="1">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="10"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
     </row>
     <row r="17" ht="13.5" customHeight="1">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="10"/>
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
     </row>
     <row r="18" ht="13.5" customHeight="1">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="10"/>
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
     </row>
     <row r="19" ht="15.95" customHeight="1">
       <c r="A19" s="20"/>

</xml_diff>

<commit_message>
Enable User to download and edit NGS measurement data  (#545)
* Enable measurement metadata download dependent on selected tab

* Enable Editing for NGS measurement spreadsheet

* Fix Tests

* Enable editing of NGS measurements

* Add JD

* Set proper capitalization of processes and set measurement number correctly

* Reload measurements after successful edit and registration

* Fix pooling for registration and move pooling group to beginning of ngs template

* Fix Validation for NGS and Proteomics Update to also check validity of RoR and InstrumentId

* Fix styling of columns within the ngs downloaded measurment file

* Ensure that all measurements are updated correctly during edit

* Remove domain model dependency from application service

* Adjust methods since aggregate does not implement MeasurementMetadata anymore

---------

Co-authored-by: Sven Fillinger <sven.fillinger@qbic.uni-tuebingen.de>
</commit_message>
<xml_diff>
--- a/user-interface/src/main/resources/templates/ngs_measurement_registration_sheet.xlsx
+++ b/user-interface/src/main/resources/templates/ngs_measurement_registration_sheet.xlsx
@@ -21,6 +21,9 @@
     <t>Sample Label</t>
   </si>
   <si>
+    <t>Sample Pool Group</t>
+  </si>
+  <si>
     <t>Organisation id*</t>
   </si>
   <si>
@@ -42,9 +45,6 @@
     <t>Sequencing run protocol</t>
   </si>
   <si>
-    <t>Sample Pool Group</t>
-  </si>
-  <si>
     <t>Index i7</t>
   </si>
   <si>
@@ -78,6 +78,9 @@
     <t>This is just a visual aid simplify sample navigation. This column gets ignored during measurement registration</t>
   </si>
   <si>
+    <t>In case of pooled sample get measured, indicate with a common sample group label for samples that are in the same measurement. Entries that share the same pool label will be combined as one measurement</t>
+  </si>
+  <si>
     <t>Organisation id</t>
   </si>
   <si>
@@ -111,9 +114,6 @@
     <t>Information on how many cycles for each read and index</t>
   </si>
   <si>
-    <t>In case of pooled sample get measured, indicate with a common sample group label for samples that are in the same measurement. Entries that share the same pool label will be combined as one measurement</t>
-  </si>
-  <si>
     <t>Index used for multiplexing</t>
   </si>
   <si>
@@ -126,6 +126,9 @@
     <t>Free text</t>
   </si>
   <si>
+    <t>number (e.g. 1, 2, 3)</t>
+  </si>
+  <si>
     <t>full ROR url</t>
   </si>
   <si>
@@ -133,9 +136,6 @@
   </si>
   <si>
     <t xml:space="preserve">ontology CURIE (e.g. EFO:0008637) </t>
-  </si>
-  <si>
-    <t>number (e.g. 1, 2, 3)</t>
   </si>
   <si>
     <t>free text (max. 500 characters)</t>
@@ -309,19 +309,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -1412,12 +1412,14 @@
   <sheetFormatPr defaultColWidth="10.8333" defaultRowHeight="15.95" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="29.1719" style="1" customWidth="1"/>
-    <col min="2" max="3" width="23.6719" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.8516" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.5" style="1" customWidth="1"/>
-    <col min="7" max="8" width="10.8516" style="1" customWidth="1"/>
-    <col min="9" max="10" width="26" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23.6719" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.6719" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.8516" style="1" customWidth="1"/>
+    <col min="7" max="7" width="22.5" style="1" customWidth="1"/>
+    <col min="8" max="9" width="10.8516" style="1" customWidth="1"/>
+    <col min="10" max="10" width="26" style="1" customWidth="1"/>
     <col min="11" max="12" width="10.8516" style="1" customWidth="1"/>
     <col min="13" max="13" width="101.352" style="1" customWidth="1"/>
     <col min="14" max="16384" width="10.8516" style="1" customWidth="1"/>
@@ -1467,14 +1469,14 @@
     <row r="2" ht="17.1" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
+      <c r="C2" s="4"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
-      <c r="J2" s="4"/>
+      <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
@@ -1482,14 +1484,14 @@
     <row r="3" ht="17.1" customHeight="1">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
+      <c r="C3" s="4"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
-      <c r="J3" s="4"/>
+      <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
@@ -1497,14 +1499,14 @@
     <row r="4" ht="17.1" customHeight="1">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
+      <c r="C4" s="4"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
-      <c r="J4" s="4"/>
+      <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
@@ -1512,14 +1514,14 @@
     <row r="5" ht="17.1" customHeight="1">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
+      <c r="C5" s="4"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
-      <c r="J5" s="4"/>
+      <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
@@ -1527,14 +1529,14 @@
     <row r="6" ht="17.1" customHeight="1">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
+      <c r="C6" s="4"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
-      <c r="J6" s="4"/>
+      <c r="J6" s="3"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
@@ -1542,14 +1544,14 @@
     <row r="7" ht="17.1" customHeight="1">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
+      <c r="C7" s="6"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="7"/>
       <c r="I7" s="5"/>
-      <c r="J7" s="7"/>
+      <c r="J7" s="5"/>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
@@ -1557,14 +1559,14 @@
     <row r="8" ht="17.1" customHeight="1">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
+      <c r="C8" s="9"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="10"/>
       <c r="I8" s="8"/>
-      <c r="J8" s="10"/>
+      <c r="J8" s="8"/>
       <c r="K8" s="8"/>
       <c r="L8" s="8"/>
       <c r="M8" s="8"/>
@@ -1572,14 +1574,14 @@
     <row r="9" ht="17.1" customHeight="1">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
+      <c r="C9" s="9"/>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="10"/>
       <c r="I9" s="8"/>
-      <c r="J9" s="10"/>
+      <c r="J9" s="8"/>
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
       <c r="M9" s="8"/>
@@ -1587,21 +1589,21 @@
     <row r="10" ht="17.1" customHeight="1">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
+      <c r="C10" s="9"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="10"/>
       <c r="I10" s="8"/>
-      <c r="J10" s="10"/>
+      <c r="J10" s="8"/>
       <c r="K10" s="8"/>
       <c r="L10" s="8"/>
       <c r="M10" s="8"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F7:F10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G7:G10">
       <formula1>"single-end,paired-end"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1666,64 +1668,64 @@
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
     </row>
-    <row r="4" ht="26.65" customHeight="1">
+    <row r="4" ht="17.1" customHeight="1">
       <c r="A4" t="s" s="13">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s" s="13">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s" s="14">
         <v>21</v>
-      </c>
-      <c r="B4" t="s" s="13">
-        <v>17</v>
-      </c>
-      <c r="C4" t="s" s="14">
-        <v>22</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" ht="17.1" customHeight="1">
+    <row r="5" ht="26.65" customHeight="1">
       <c r="A5" t="s" s="13">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s" s="13">
         <v>17</v>
       </c>
       <c r="C5" t="s" s="14">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
     </row>
-    <row r="6" ht="39.6" customHeight="1">
+    <row r="6" ht="17.1" customHeight="1">
       <c r="A6" t="s" s="13">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s" s="13">
         <v>17</v>
       </c>
       <c r="C6" t="s" s="14">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
     </row>
-    <row r="7" ht="17.1" customHeight="1">
+    <row r="7" ht="39.6" customHeight="1">
       <c r="A7" t="s" s="13">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s" s="13">
         <v>17</v>
       </c>
       <c r="C7" t="s" s="14">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
     </row>
-    <row r="8" ht="26.65" customHeight="1">
+    <row r="8" ht="17.1" customHeight="1">
       <c r="A8" t="s" s="13">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s" s="13">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s" s="14">
         <v>29</v>
@@ -1731,7 +1733,7 @@
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
     </row>
-    <row r="9" ht="17.1" customHeight="1">
+    <row r="9" ht="26.65" customHeight="1">
       <c r="A9" t="s" s="13">
         <v>7</v>
       </c>
@@ -1827,14 +1829,15 @@
   <sheetFormatPr defaultColWidth="10.8333" defaultRowHeight="15.95" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="30.3516" style="15" customWidth="1"/>
-    <col min="2" max="3" width="16" style="15" customWidth="1"/>
-    <col min="4" max="4" width="18.6719" style="15" customWidth="1"/>
-    <col min="5" max="5" width="35.8516" style="15" customWidth="1"/>
-    <col min="6" max="6" width="26.6719" style="15" customWidth="1"/>
-    <col min="7" max="7" width="15.3516" style="15" customWidth="1"/>
-    <col min="8" max="8" width="14.8516" style="15" customWidth="1"/>
-    <col min="9" max="9" width="22.8516" style="15" customWidth="1"/>
-    <col min="10" max="10" width="19.1719" style="15" customWidth="1"/>
+    <col min="2" max="2" width="16" style="15" customWidth="1"/>
+    <col min="3" max="3" width="19.1719" style="15" customWidth="1"/>
+    <col min="4" max="4" width="16" style="15" customWidth="1"/>
+    <col min="5" max="5" width="18.6719" style="15" customWidth="1"/>
+    <col min="6" max="6" width="35.8516" style="15" customWidth="1"/>
+    <col min="7" max="7" width="26.6719" style="15" customWidth="1"/>
+    <col min="8" max="8" width="15.3516" style="15" customWidth="1"/>
+    <col min="9" max="9" width="14.8516" style="15" customWidth="1"/>
+    <col min="10" max="10" width="22.8516" style="15" customWidth="1"/>
     <col min="11" max="12" width="16.6719" style="15" customWidth="1"/>
     <col min="13" max="13" width="24" style="15" customWidth="1"/>
     <col min="14" max="16384" width="10.8516" style="15" customWidth="1"/>
@@ -1856,10 +1859,10 @@
       <c r="E1" t="s" s="2">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="16">
+      <c r="F1" t="s" s="2">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="2">
+      <c r="G1" t="s" s="16">
         <v>6</v>
       </c>
       <c r="H1" t="s" s="2">
@@ -1888,7 +1891,7 @@
       <c r="B2" t="s" s="17">
         <v>36</v>
       </c>
-      <c r="C2" t="s" s="17">
+      <c r="C2" t="s" s="18">
         <v>37</v>
       </c>
       <c r="D2" t="s" s="17">
@@ -1897,10 +1900,10 @@
       <c r="E2" t="s" s="17">
         <v>39</v>
       </c>
-      <c r="F2" t="s" s="13">
-        <v>36</v>
-      </c>
-      <c r="G2" t="s" s="17">
+      <c r="F2" t="s" s="17">
+        <v>40</v>
+      </c>
+      <c r="G2" t="s" s="13">
         <v>36</v>
       </c>
       <c r="H2" t="s" s="17">
@@ -1909,8 +1912,8 @@
       <c r="I2" t="s" s="17">
         <v>36</v>
       </c>
-      <c r="J2" t="s" s="18">
-        <v>40</v>
+      <c r="J2" t="s" s="17">
+        <v>36</v>
       </c>
       <c r="K2" t="s" s="17">
         <v>36</v>
@@ -1927,250 +1930,250 @@
         <v>42</v>
       </c>
       <c r="B3" s="13"/>
-      <c r="C3" t="s" s="13">
+      <c r="C3" s="13"/>
+      <c r="D3" t="s" s="13">
         <v>43</v>
       </c>
-      <c r="D3" s="10"/>
-      <c r="E3" t="s" s="13">
+      <c r="E3" s="9"/>
+      <c r="F3" t="s" s="13">
         <v>44</v>
       </c>
-      <c r="F3" s="13"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
     </row>
     <row r="4" ht="13.5" customHeight="1">
-      <c r="A4" s="10"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" t="s" s="13">
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" t="s" s="13">
         <v>45</v>
       </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
       <c r="M4" s="19"/>
     </row>
     <row r="5" ht="13.5" customHeight="1">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" t="s" s="13">
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" t="s" s="13">
         <v>46</v>
       </c>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
     </row>
     <row r="6" ht="13.5" customHeight="1">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
     </row>
     <row r="7" ht="13.5" customHeight="1">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
     </row>
     <row r="8" ht="13.5" customHeight="1">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
     </row>
     <row r="9" ht="13.5" customHeight="1">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
     </row>
     <row r="10" ht="13.5" customHeight="1">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
     </row>
     <row r="11" ht="13.5" customHeight="1">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
     </row>
     <row r="12" ht="13.5" customHeight="1">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
     </row>
     <row r="13" ht="13.5" customHeight="1">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
     </row>
     <row r="14" ht="13.5" customHeight="1">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
     </row>
     <row r="15" ht="13.5" customHeight="1">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
     </row>
     <row r="16" ht="13.5" customHeight="1">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="10"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
     </row>
     <row r="17" ht="13.5" customHeight="1">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="10"/>
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
     </row>
     <row r="18" ht="13.5" customHeight="1">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="10"/>
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
     </row>
     <row r="19" ht="15.95" customHeight="1">
       <c r="A19" s="20"/>

</xml_diff>

<commit_message>
rename sample label to sample name
</commit_message>
<xml_diff>
--- a/user-interface/src/main/resources/templates/ngs_measurement_registration_sheet.xlsx
+++ b/user-interface/src/main/resources/templates/ngs_measurement_registration_sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sven1103/git/data-manager/user-interface/src/main/resources/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/afriedrich/git/data-manager-app/user-interface/src/main/resources/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64FC47CD-9AAC-904D-8116-A4CC2F34B820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A78CB178-6959-4249-A3DE-1D39E283EB49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -26,9 +26,6 @@
     <t>QBIC sample id*</t>
   </si>
   <si>
-    <t>Sample Label</t>
-  </si>
-  <si>
     <t>Sample Pool Group</t>
   </si>
   <si>
@@ -126,13 +123,16 @@
   </si>
   <si>
     <t>Commenting notes about the measurement (max 500 characters)</t>
+  </si>
+  <si>
+    <t>Sample Name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -1397,11 +1397,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.1640625" style="4" bestFit="1" customWidth="1"/>
@@ -1419,48 +1419,48 @@
     <col min="15" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="6"/>
@@ -1475,7 +1475,7 @@
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
@@ -1490,7 +1490,7 @@
       <c r="L3" s="5"/>
       <c r="M3" s="5"/>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="6"/>
@@ -1505,7 +1505,7 @@
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="6"/>
@@ -1520,7 +1520,7 @@
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="6"/>
@@ -1535,7 +1535,7 @@
       <c r="L6" s="5"/>
       <c r="M6" s="5"/>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="8"/>
@@ -1550,7 +1550,7 @@
       <c r="L7" s="7"/>
       <c r="M7" s="7"/>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="10"/>
       <c r="B8" s="10"/>
       <c r="C8" s="11"/>
@@ -1565,7 +1565,7 @@
       <c r="L8" s="10"/>
       <c r="M8" s="10"/>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="10"/>
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
@@ -1580,7 +1580,7 @@
       <c r="L9" s="10"/>
       <c r="M9" s="10"/>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="10"/>
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
@@ -1613,11 +1613,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
@@ -1627,226 +1627,226 @@
     <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="C1" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="13" t="s">
         <v>14</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>15</v>
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" ht="20">
+    <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="14" t="s">
         <v>16</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>17</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" ht="40">
+    <row r="3" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="B3" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="14" t="s">
         <v>18</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>19</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" ht="60">
+    <row r="4" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6" ht="60">
+    <row r="5" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:6" ht="20">
+    <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:6" ht="80">
+    <row r="7" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:6" ht="20">
+    <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:6" ht="40">
+    <row r="9" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:6" ht="20">
+    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" ht="20">
+    <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" ht="20">
+    <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:6" ht="20">
+    <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" ht="20">
+    <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>

</xml_diff>

<commit_message>
Change cursor position to first row first sample
</commit_message>
<xml_diff>
--- a/user-interface/src/main/resources/templates/ngs_measurement_registration_sheet.xlsx
+++ b/user-interface/src/main/resources/templates/ngs_measurement_registration_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kocht/SoftwareDevelopment/portlets/data-manager-app/user-interface/src/main/resources/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4379BACA-F62F-9A40-8B9F-F94ED5CC0C2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A6C7429-CBB6-CB45-952F-8145BB38106B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1398,7 +1398,7 @@
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19"/>

</xml_diff>

<commit_message>
Fix NGS measurement template dropdowns (#828)
* fix template

* Change cursor position to first row first sample

* update dev.bundle
</commit_message>
<xml_diff>
--- a/user-interface/src/main/resources/templates/ngs_measurement_registration_sheet.xlsx
+++ b/user-interface/src/main/resources/templates/ngs_measurement_registration_sheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/afriedrich/git/data-manager-app/user-interface/src/main/resources/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kocht/SoftwareDevelopment/portlets/data-manager-app/user-interface/src/main/resources/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A78CB178-6959-4249-A3DE-1D39E283EB49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A6C7429-CBB6-CB45-952F-8145BB38106B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -132,7 +132,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -1398,10 +1398,10 @@
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19"/>
   <cols>
     <col min="1" max="1" width="15.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.1640625" style="4" bestFit="1" customWidth="1"/>
@@ -1419,7 +1419,7 @@
     <col min="15" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1460,14 +1460,14 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="6"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
+      <c r="G2" s="7"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
@@ -1475,14 +1475,14 @@
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
+      <c r="G3" s="7"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
@@ -1490,14 +1490,14 @@
       <c r="L3" s="5"/>
       <c r="M3" s="5"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="6"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
+      <c r="G4" s="7"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
@@ -1505,14 +1505,14 @@
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="6"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
+      <c r="G5" s="7"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
@@ -1520,14 +1520,14 @@
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="6"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
+      <c r="G6" s="7"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
@@ -1535,7 +1535,7 @@
       <c r="L6" s="5"/>
       <c r="M6" s="5"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="8"/>
@@ -1550,7 +1550,7 @@
       <c r="L7" s="7"/>
       <c r="M7" s="7"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13">
       <c r="A8" s="10"/>
       <c r="B8" s="10"/>
       <c r="C8" s="11"/>
@@ -1565,7 +1565,7 @@
       <c r="L8" s="10"/>
       <c r="M8" s="10"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13">
       <c r="A9" s="10"/>
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
@@ -1580,7 +1580,7 @@
       <c r="L9" s="10"/>
       <c r="M9" s="10"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13">
       <c r="A10" s="10"/>
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
@@ -1597,7 +1597,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G7:G10" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G10" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"single-end,paired-end"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1617,7 +1617,7 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="24.5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
@@ -1627,7 +1627,7 @@
     <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="19">
       <c r="A1" s="13" t="s">
         <v>12</v>
       </c>
@@ -1643,7 +1643,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="20">
       <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
@@ -1659,7 +1659,7 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="40">
       <c r="A3" s="12" t="s">
         <v>34</v>
       </c>
@@ -1675,7 +1675,7 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="60">
       <c r="A4" s="12" t="s">
         <v>1</v>
       </c>
@@ -1691,7 +1691,7 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="60">
       <c r="A5" s="12" t="s">
         <v>2</v>
       </c>
@@ -1707,7 +1707,7 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="20">
       <c r="A6" s="12" t="s">
         <v>3</v>
       </c>
@@ -1723,7 +1723,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="80">
       <c r="A7" s="12" t="s">
         <v>4</v>
       </c>
@@ -1739,7 +1739,7 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="20">
       <c r="A8" s="12" t="s">
         <v>5</v>
       </c>
@@ -1755,7 +1755,7 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="40">
       <c r="A9" s="12" t="s">
         <v>6</v>
       </c>
@@ -1771,7 +1771,7 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="20">
       <c r="A10" s="12" t="s">
         <v>7</v>
       </c>
@@ -1787,7 +1787,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="20">
       <c r="A11" s="12" t="s">
         <v>8</v>
       </c>
@@ -1803,7 +1803,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="20">
       <c r="A12" s="12" t="s">
         <v>9</v>
       </c>
@@ -1819,7 +1819,7 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="20">
       <c r="A13" s="12" t="s">
         <v>10</v>
       </c>
@@ -1835,7 +1835,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="20">
       <c r="A14" s="12" t="s">
         <v>11</v>
       </c>

</xml_diff>